<commit_message>
update graphs and antibiotic discovery timeline
</commit_message>
<xml_diff>
--- a/antibiotic-discovery/antibiotic-discovery.xlsx
+++ b/antibiotic-discovery/antibiotic-discovery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4399efb1e589f8b/Documents/GitHub/phd-chapter3-2024/antibiotic-discovery/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1crh\Documents\GitHub\phd-chapter3-4-2024\antibiotic-discovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{E631FB1B-80C0-43DC-82AB-129F7427A459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F091C5D7-BABA-4FF6-B779-113FB71B724F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8F6191-A2B9-42CA-A819-BFB9E0864EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Arsphenamines</t>
   </si>
@@ -51,15 +51,6 @@
     <t>Oxazolidinones</t>
   </si>
   <si>
-    <t>Ansamycins</t>
-  </si>
-  <si>
-    <t>Quinolones</t>
-  </si>
-  <si>
-    <t>Lincosamides</t>
-  </si>
-  <si>
     <t>class</t>
   </si>
   <si>
@@ -72,10 +63,25 @@
     <t>timeline</t>
   </si>
   <si>
-    <t>Phenicols and Lipopeptides</t>
-  </si>
-  <si>
-    <t>Glycopeptides and Streptogramins</t>
+    <t>Phenicols</t>
+  </si>
+  <si>
+    <t>Glycopeptides</t>
+  </si>
+  <si>
+    <t>Streptogramins</t>
+  </si>
+  <si>
+    <t>Azoles</t>
+  </si>
+  <si>
+    <t>Quinolones and Lincosamides</t>
+  </si>
+  <si>
+    <t>Diarylquinolines</t>
+  </si>
+  <si>
+    <t>Nitrofurans</t>
   </si>
 </sst>
 </file>
@@ -129,10 +135,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,13 +414,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -426,10 +428,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>3654</v>
+        <v>2558</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -440,7 +442,7 @@
         <v>10594</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -448,10 +450,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>12785</v>
+        <v>11689</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -462,7 +464,7 @@
         <v>14246</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -470,98 +472,120 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>15707</v>
+        <v>16072</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
         <v>16438</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>17168</v>
+        <v>17533</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1">
-        <v>18264</v>
+        <v>17168</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>18994</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
         <v>19360</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>20821</v>
+        <v>19725</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>22647</v>
+        <v>21551</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>23012</v>
+        <v>22647</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1">
+        <v>31778</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>37987</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>